<commit_message>
Add update clean data.
</commit_message>
<xml_diff>
--- a/p1/clean data.xlsx
+++ b/p1/clean data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vayne-Lover\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vayne-Lover\Desktop\p1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Help prepare for an advanced degree</t>
   </si>
@@ -76,10 +76,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Recommand</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Associates</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -89,6 +85,36 @@
   </si>
   <si>
     <t>Highest level of education</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>Hours</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sitting per day</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -721,6 +747,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-07C3-4A14-8280-32DE85DD738D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -740,6 +771,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-07C3-4A14-8280-32DE85DD738D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -936,490 +972,6 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Recommended possibility</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$Q$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Numbers</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:alpha val="70000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="110000"/>
-                      <a:satMod val="105000"/>
-                      <a:tint val="67000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="105000"/>
-                      <a:satMod val="103000"/>
-                      <a:tint val="73000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="105000"/>
-                      <a:satMod val="109000"/>
-                      <a:tint val="81000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:shade val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="18000" rIns="0" bIns="0" anchor="ctr" anchorCtr="0">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <a:prstGeom prst="rect">
-                    <a:avLst/>
-                  </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                </c15:spPr>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="rnd">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$P$2:$P$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$Q$2:$Q$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>147</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>378</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A47D-4113-8CFE-4FAE24548B79}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1371047327"/>
-        <c:axId val="1339531087"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1371047327"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="10"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="20000"/>
-                <a:lumOff val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1339531087"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1339531087"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1371047327"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:alpha val="0"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
@@ -1934,46 +1486,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="204">
   <cs:axisTitle>
@@ -3073,557 +2585,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4269,42 +3230,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FDF400E-425D-4898-9F0B-492ABA8BA070}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>7</xdr:row>
@@ -4333,7 +3258,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4350,7 +3275,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -4639,10 +3564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D26BB0-F285-4CDD-B08C-30563CD71974}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
@@ -4654,12 +3579,12 @@
     <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -4673,19 +3598,19 @@
         <v>10</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4704,14 +3629,14 @@
       <c r="K2" s="2">
         <v>45</v>
       </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>2</v>
+      <c r="Q2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="2">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4730,14 +3655,14 @@
       <c r="K3" s="2">
         <v>24</v>
       </c>
-      <c r="P3" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>1</v>
+      <c r="Q3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="2">
+        <v>9.6455525606468999</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -4745,19 +3670,19 @@
         <v>88</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="2">
         <v>12</v>
       </c>
-      <c r="P4" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>4</v>
+      <c r="Q4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="2">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -4770,14 +3695,14 @@
       <c r="K5" s="2">
         <v>283</v>
       </c>
-      <c r="P5" s="2">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>10</v>
+      <c r="Q5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="2">
+        <v>2.9742335358783745</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -4785,19 +3710,19 @@
         <v>411</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" s="2">
         <v>316</v>
       </c>
-      <c r="P6" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -4810,35 +3735,19 @@
       <c r="K7" s="2">
         <v>73</v>
       </c>
-      <c r="P7" s="2">
-        <v>7</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>59</v>
+      <c r="Q7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="P8" s="2">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="P9" s="2">
-        <v>9</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="P10" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>378</v>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R8" s="2">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>